<commit_message>
Feat / add def to loop DF
</commit_message>
<xml_diff>
--- a/panda-env/src/Notes.xlsx
+++ b/panda-env/src/Notes.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Python course\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Python course\panda-env\src\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FBE97C1-2087-4436-B1B1-106DA21CABF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F8395A6-C908-44BC-90AA-D99C84A34A97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -507,16 +507,16 @@
     <t>Name</t>
   </si>
   <si>
-    <t>Note Period |</t>
-  </si>
-  <si>
-    <t>Note Period ||</t>
-  </si>
-  <si>
-    <t>Note Period |||</t>
-  </si>
-  <si>
-    <t>Note Period  IV</t>
+    <t>Grade1</t>
+  </si>
+  <si>
+    <t>Grade2</t>
+  </si>
+  <si>
+    <t>Grade3</t>
+  </si>
+  <si>
+    <t>Grade4</t>
   </si>
 </sst>
 </file>
@@ -1065,7 +1065,7 @@
   <dimension ref="A1:F115"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:H5"/>
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5703125" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>